<commit_message>
Update cost data with LCOE and variable cost only
Update cost data with LCOE and variable cost only
</commit_message>
<xml_diff>
--- a/WECC_NPCC_Systems/Cost/Cost.xlsx
+++ b/WECC_NPCC_Systems/Cost/Cost.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\qzhan\Dropbox\Idea\under progress\Pmarket\System\form\fuel data\final_file\WECC_NPCC_Systems\Cost\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\qzhan\Dropbox\Idea\under progress\Pmarket\System\form\fuel data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AE3DB81-6962-4FBA-9C72-8EE47E8851CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DC0ADE9-52A2-4F2C-BD61-E58660C832E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23660" yWindow="4250" windowWidth="28770" windowHeight="15590" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13040" yWindow="4190" windowWidth="21570" windowHeight="15220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WECC" sheetId="1" r:id="rId1"/>
@@ -355,12 +355,12 @@
   <dimension ref="A1:C30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -371,7 +371,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -379,10 +379,10 @@
         <v>27.206068399999999</v>
       </c>
       <c r="C2">
-        <v>14146.659799999999</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -390,10 +390,10 @@
         <v>25.371083299999999</v>
       </c>
       <c r="C3">
-        <v>11356.974700000001</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -401,10 +401,10 @@
         <v>24.2798041</v>
       </c>
       <c r="C4">
-        <v>9889.2133599999997</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -412,10 +412,10 @@
         <v>18.029580500000002</v>
       </c>
       <c r="C5">
-        <v>7936.9187400000001</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -423,10 +423,10 @@
         <v>22.7843236</v>
       </c>
       <c r="C6">
-        <v>5221.9475899999998</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -434,10 +434,10 @@
         <v>4.4686514700000002</v>
       </c>
       <c r="C7">
-        <v>39140.812400000003</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -445,10 +445,10 @@
         <v>24.726170499999998</v>
       </c>
       <c r="C8">
-        <v>11721.393</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -459,7 +459,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -470,7 +470,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -478,10 +478,10 @@
         <v>25.107340099999998</v>
       </c>
       <c r="C11">
-        <v>12168.610199999999</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -489,10 +489,10 @@
         <v>17.707898799999999</v>
       </c>
       <c r="C12">
-        <v>4681.1109900000001</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
@@ -500,10 +500,10 @@
         <v>22.314001300000001</v>
       </c>
       <c r="C13">
-        <v>4047.0055200000002</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
@@ -511,10 +511,10 @@
         <v>21.085790100000001</v>
       </c>
       <c r="C14">
-        <v>17618.287400000001</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
@@ -522,10 +522,10 @@
         <v>10.9259635</v>
       </c>
       <c r="C15">
-        <v>10608.4668</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
@@ -533,10 +533,10 @@
         <v>12.779708100000001</v>
       </c>
       <c r="C16">
-        <v>4103.2040900000002</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
@@ -544,10 +544,10 @@
         <v>0</v>
       </c>
       <c r="C17">
-        <v>11209.6729</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
@@ -555,10 +555,10 @@
         <v>15.275318</v>
       </c>
       <c r="C18">
-        <v>4113.4932099999996</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>18</v>
       </c>
@@ -566,10 +566,10 @@
         <v>4.8053730200000002</v>
       </c>
       <c r="C19">
-        <v>10832.001899999999</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>19</v>
       </c>
@@ -577,10 +577,10 @@
         <v>1.98505061</v>
       </c>
       <c r="C20">
-        <v>24198.645199999999</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>20</v>
       </c>
@@ -588,10 +588,10 @@
         <v>15.2090268</v>
       </c>
       <c r="C21">
-        <v>4394.1464599999999</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>21</v>
       </c>
@@ -599,10 +599,10 @@
         <v>24.861268800000001</v>
       </c>
       <c r="C22">
-        <v>4440.5133900000001</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>22</v>
       </c>
@@ -610,10 +610,10 @@
         <v>0</v>
       </c>
       <c r="C23">
-        <v>3902.7815799999998</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>23</v>
       </c>
@@ -621,10 +621,10 @@
         <v>0</v>
       </c>
       <c r="C24">
-        <v>6064.7834899999998</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>24</v>
       </c>
@@ -632,10 +632,10 @@
         <v>24.619512499999999</v>
       </c>
       <c r="C25">
-        <v>3365.2932799999999</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>25</v>
       </c>
@@ -643,10 +643,10 @@
         <v>19.115309</v>
       </c>
       <c r="C26">
-        <v>8000.7104200000003</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>26</v>
       </c>
@@ -654,10 +654,10 @@
         <v>25.9148675</v>
       </c>
       <c r="C27">
-        <v>4971.07</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>27</v>
       </c>
@@ -665,10 +665,10 @@
         <v>24.334967800000001</v>
       </c>
       <c r="C28">
-        <v>4774.0898999999999</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>28</v>
       </c>
@@ -676,10 +676,10 @@
         <v>26.183388300000001</v>
       </c>
       <c r="C29">
-        <v>6921.0315300000002</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>29</v>
       </c>
@@ -687,7 +687,7 @@
         <v>25.559399200000001</v>
       </c>
       <c r="C30">
-        <v>6968.29846</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -700,12 +700,15 @@
   <dimension ref="A1:C49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="C37" sqref="C37:C49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="36.1796875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -716,7 +719,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -724,10 +727,10 @@
         <v>2.14</v>
       </c>
       <c r="C2">
-        <v>56690.134246575297</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -735,10 +738,10 @@
         <v>26.751182886906399</v>
       </c>
       <c r="C3">
-        <v>2882.8778538812799</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -746,10 +749,10 @@
         <v>29.3552649251662</v>
       </c>
       <c r="C4">
-        <v>2451.2428652968001</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -757,10 +760,10 @@
         <v>26.608680932758102</v>
       </c>
       <c r="C5">
-        <v>1318.09432077626</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -768,10 +771,10 @@
         <v>27.6659342904398</v>
       </c>
       <c r="C6">
-        <v>5385.6650684931501</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -779,10 +782,10 @@
         <v>28.7459945621735</v>
       </c>
       <c r="C7">
-        <v>2795.8110730593598</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -790,10 +793,10 @@
         <v>18.268960791298401</v>
       </c>
       <c r="C8">
-        <v>1726.7908889840201</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -801,10 +804,10 @@
         <v>8.9794433889545999</v>
       </c>
       <c r="C9">
-        <v>9438.8712043379001</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -812,10 +815,10 @@
         <v>26.5299770118196</v>
       </c>
       <c r="C10">
-        <v>3643.0998382800599</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -823,10 +826,10 @@
         <v>26.0833522820338</v>
       </c>
       <c r="C11">
-        <v>4319.9634417808202</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -834,10 +837,10 @@
         <v>0</v>
       </c>
       <c r="C12">
-        <v>4974.5973173516004</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
@@ -845,10 +848,10 @@
         <v>0</v>
       </c>
       <c r="C13">
-        <v>242.60273972602701</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
@@ -856,10 +859,10 @@
         <v>2.14</v>
       </c>
       <c r="C14">
-        <v>47967.476255707799</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
@@ -867,10 +870,10 @@
         <v>25.403933810628999</v>
       </c>
       <c r="C15">
-        <v>5153.9550799086801</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
@@ -878,10 +881,10 @@
         <v>2.14</v>
       </c>
       <c r="C16">
-        <v>19425.985045662099</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
@@ -892,7 +895,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
@@ -903,7 +906,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>18</v>
       </c>
@@ -914,7 +917,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>19</v>
       </c>
@@ -922,10 +925,10 @@
         <v>0</v>
       </c>
       <c r="C20">
-        <v>8378.8356164383604</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>20</v>
       </c>
@@ -933,10 +936,10 @@
         <v>0</v>
       </c>
       <c r="C21">
-        <v>331.91780821917803</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>21</v>
       </c>
@@ -944,10 +947,10 @@
         <v>25.0345853361124</v>
       </c>
       <c r="C22">
-        <v>3069.5345890410999</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>22</v>
       </c>
@@ -955,10 +958,10 @@
         <v>26.311591723706499</v>
       </c>
       <c r="C23">
-        <v>3912.3144977169</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>23</v>
       </c>
@@ -969,7 +972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>24</v>
       </c>
@@ -977,10 +980,10 @@
         <v>26.504175425725901</v>
       </c>
       <c r="C25">
-        <v>6348.6194349315101</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>25</v>
       </c>
@@ -988,10 +991,10 @@
         <v>2.14</v>
       </c>
       <c r="C26">
-        <v>23130.900456620999</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>26</v>
       </c>
@@ -999,10 +1002,10 @@
         <v>26.071128266555501</v>
       </c>
       <c r="C27">
-        <v>1544.4998573059399</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1010,10 +1013,10 @@
         <v>29.312622127603799</v>
       </c>
       <c r="C28">
-        <v>7266.0358447488597</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1021,10 +1024,10 @@
         <v>26.602313917034198</v>
       </c>
       <c r="C29">
-        <v>2597.66301369863</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1032,10 +1035,10 @@
         <v>33.849907862900601</v>
       </c>
       <c r="C30">
-        <v>4945.89108162101</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1043,10 +1046,10 @@
         <v>27.6411935399775</v>
       </c>
       <c r="C31">
-        <v>3083.3163955479499</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1057,7 +1060,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1068,7 +1071,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1079,7 +1082,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1090,7 +1093,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1098,10 +1101,10 @@
         <v>0</v>
       </c>
       <c r="C36">
-        <v>2860.5468036529701</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1112,7 +1115,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1120,10 +1123,10 @@
         <v>26.686902889577599</v>
       </c>
       <c r="C38">
-        <v>5688.3630136986303</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1131,10 +1134,10 @@
         <v>25.812028432753401</v>
       </c>
       <c r="C39">
-        <v>6524.5884703196298</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>39</v>
       </c>
@@ -1142,10 +1145,10 @@
         <v>2.14</v>
       </c>
       <c r="C40">
-        <v>57144.552442922402</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>40</v>
       </c>
@@ -1153,10 +1156,10 @@
         <v>14.4354407472362</v>
       </c>
       <c r="C41">
-        <v>18141.341438356201</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>41</v>
       </c>
@@ -1164,10 +1167,10 @@
         <v>39.426395627431198</v>
       </c>
       <c r="C42">
-        <v>11883.0015410959</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>42</v>
       </c>
@@ -1175,10 +1178,10 @@
         <v>17.008008837434701</v>
       </c>
       <c r="C43">
-        <v>37093.713727168899</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>43</v>
       </c>
@@ -1186,10 +1189,10 @@
         <v>2.14</v>
       </c>
       <c r="C44">
-        <v>77390.0044931507</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>44</v>
       </c>
@@ -1197,10 +1200,10 @@
         <v>9.7126220004342496</v>
       </c>
       <c r="C45">
-        <v>32840.146033104997</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>45</v>
       </c>
@@ -1208,10 +1211,10 @@
         <v>7.2306862685262603</v>
       </c>
       <c r="C46">
-        <v>36528.826917808197</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>46</v>
       </c>
@@ -1219,10 +1222,10 @@
         <v>22.1102515396061</v>
       </c>
       <c r="C47">
-        <v>13727.471575342501</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>47</v>
       </c>
@@ -1230,10 +1233,10 @@
         <v>25.139279307249002</v>
       </c>
       <c r="C48">
-        <v>6491.5967465753401</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>48</v>
       </c>
@@ -1241,7 +1244,7 @@
         <v>19.6324470075512</v>
       </c>
       <c r="C49">
-        <v>35838.983219178102</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>